<commit_message>
Restructuralized files, removed unused diagrams, added CD/DVD content
</commit_message>
<xml_diff>
--- a/Text/diagrams/PerformanceChartComparePrototypeAndFinal.xlsx
+++ b/Text/diagrams/PerformanceChartComparePrototypeAndFinal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VUT FIT\10. semestr\DIP\Diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Josefik\Master-Thesis\Text\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECBC48C-BA09-4C17-9966-4D991181D938}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73633D09-938B-4711-8FC3-BF8BFACAD862}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" xr2:uid="{0731F486-61CF-4A44-ADA1-383D3BC3EEA7}"/>
   </bookViews>
@@ -25,24 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Count</t>
   </si>
   <si>
     <t>Time (s)</t>
-  </si>
-  <si>
-    <t>dns.pcap</t>
-  </si>
-  <si>
-    <t>sip_rtp.pcap</t>
-  </si>
-  <si>
-    <t>SkypeIRC.cap</t>
-  </si>
-  <si>
-    <t>netflow.pcap</t>
   </si>
   <si>
     <t>Improved</t>
@@ -1453,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC3B40FE-9945-4C42-B064-0091A412B86C}">
-  <dimension ref="D4:H9"/>
+  <dimension ref="E4:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,7 +1452,7 @@
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>0</v>
       </c>
@@ -1475,13 +1463,10 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E5">
         <v>382</v>
       </c>
@@ -1496,10 +1481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E6">
         <v>1360</v>
       </c>
@@ -1514,10 +1496,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E7">
         <v>1879</v>
       </c>
@@ -1532,10 +1511,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E8">
         <v>2263</v>
       </c>
@@ -1550,7 +1526,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>2563</v>
       </c>

</xml_diff>